<commit_message>
refine base to adapt ngnix redirect
</commit_message>
<xml_diff>
--- a/datadesign/clubs.xlsx
+++ b/datadesign/clubs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="clubs" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="officers" sheetId="3" r:id="rId3"/>
     <sheet name="CC" sheetId="4" r:id="rId4"/>
     <sheet name="CL" sheetId="5" r:id="rId5"/>
+    <sheet name="members" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">CC!$A$1:$D$1</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="114">
   <si>
     <t>clubId</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -437,6 +438,10 @@
   </si>
   <si>
     <t xml:space="preserve">team building </t>
+  </si>
+  <si>
+    <t>mem</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -938,7 +943,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1146,7 +1151,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1300,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1948,4 +1953,23 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>